<commit_message>
Add Client ID and Client Secret
</commit_message>
<xml_diff>
--- a/input_file_templates/ez_register_direct.xlsx
+++ b/input_file_templates/ez_register_direct.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neparaka/Downloads/sl_input_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neparaka/github.com/ios-xr/ez-register/input_file_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0615102C-C37B-4C48-8582-7FC0D5DCB3C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3A16BF-1D15-0241-9D49-C5C66803A4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20080" xr2:uid="{5CF37660-FCC0-2049-BD15-CBCF19B2C5BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{5CF37660-FCC0-2049-BD15-CBCF19B2C5BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Token Export Controlled</t>
+  </si>
+  <si>
+    <t>Client ID</t>
+  </si>
+  <si>
+    <t>Client Secret</t>
   </si>
 </sst>
 </file>
@@ -428,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8540DFE0-6857-4249-9FD7-30F047331D0B}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
+      <selection activeCell="J1" sqref="J1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,9 +451,11 @@
     <col min="7" max="7" width="17.1640625" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
     <col min="9" max="9" width="25.83203125" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -475,8 +483,14 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -487,7 +501,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
     </row>

</xml_diff>